<commit_message>
added sol to test_task 0315160124
</commit_message>
<xml_diff>
--- a/AirwayData.xlsx
+++ b/AirwayData.xlsx
@@ -12,24 +12,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>Carrier</t>
+    <t>Авиа оператор</t>
   </si>
   <si>
-    <t>Flight Time (hours)</t>
+    <t>Минимальное время полета между Владивосток и Тель-Авив</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>6.50</t>
   </si>
   <si>
     <t>TK</t>
   </si>
   <si>
-    <t>S7</t>
-  </si>
-  <si>
-    <t>SU</t>
+    <t>5.83</t>
   </si>
   <si>
     <t>BA</t>
+  </si>
+  <si>
+    <t>8.08</t>
+  </si>
+  <si>
+    <t>Разница между средней ценой и медианой для полета между Владивосток и Тель-Авив</t>
+  </si>
+  <si>
+    <t>Средняя цена</t>
+  </si>
+  <si>
+    <t>Медиана</t>
+  </si>
+  <si>
+    <t>460.0</t>
+  </si>
+  <si>
+    <t>13960.0</t>
+  </si>
+  <si>
+    <t>13500.0</t>
   </si>
 </sst>
 </file>
@@ -74,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -92,80 +122,54 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
-        <v>5.833333333333333</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
-      <c r="B3" t="n">
-        <v>6.5</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
-      <c r="B4" t="n">
-        <v>6.0</v>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
-      <c r="B5" t="n">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>8.083333333333334</v>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
-      <c r="B7" t="n">
-        <v>9.75</v>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
-      <c r="B8" t="n">
-        <v>6.583333333333333</v>
+      <c r="B8" t="s">
+        <v>14</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="n">
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="n">
-        <v>10.083333333333334</v>
+      <c r="C8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added fix all 2049160124
</commit_message>
<xml_diff>
--- a/AirwayData.xlsx
+++ b/AirwayData.xlsx
@@ -6,60 +6,66 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AirwayData" r:id="rId3" sheetId="1"/>
+    <sheet name="Data and Statistics" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>Авиа оператор</t>
+    <t>Carrier</t>
   </si>
   <si>
-    <t>Минимальное время полета между Владивосток и Тель-Авив</t>
+    <t>Time Flight</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>05:50</t>
   </si>
   <si>
     <t>SU</t>
   </si>
   <si>
-    <t>6.00</t>
+    <t>06:00</t>
   </si>
   <si>
     <t>S7</t>
   </si>
   <si>
-    <t>6.50</t>
-  </si>
-  <si>
-    <t>TK</t>
-  </si>
-  <si>
-    <t>5.83</t>
+    <t>06:30</t>
   </si>
   <si>
     <t>BA</t>
   </si>
   <si>
-    <t>8.08</t>
+    <t>08:05</t>
   </si>
   <si>
-    <t>Разница между средней ценой и медианой для полета между Владивосток и Тель-Авив</t>
+    <t>Statistic</t>
   </si>
   <si>
-    <t>Средняя цена</t>
+    <t>Value</t>
   </si>
   <si>
-    <t>Медиана</t>
+    <t>Difference</t>
   </si>
   <si>
-    <t>460.0</t>
+    <t>650.00</t>
   </si>
   <si>
-    <t>13960.0</t>
+    <t>Median</t>
   </si>
   <si>
-    <t>13500.0</t>
+    <t>14200.00</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>13550.00</t>
   </si>
 </sst>
 </file>
@@ -104,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -150,26 +156,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B10" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added fix calc StatisticsPrice 1320170124
</commit_message>
<xml_diff>
--- a/AirwayData.xlsx
+++ b/AirwayData.xlsx
@@ -50,22 +50,22 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>13960.00</t>
+  </si>
+  <si>
     <t>Median</t>
   </si>
   <si>
-    <t>14200.00</t>
+    <t>13500.00</t>
   </si>
   <si>
     <t>Difference</t>
   </si>
   <si>
-    <t>650.00</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>13550.00</t>
+    <t>460.00</t>
   </si>
 </sst>
 </file>

</xml_diff>